<commit_message>
Added conclusion to Excel Sheets
</commit_message>
<xml_diff>
--- a/RMPP/Exe 8.1B.xlsx
+++ b/RMPP/Exe 8.1B.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianwolloff/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianwolloff/Desktop/MyPortfolio/RMPP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B637412A-1C61-E748-8DC6-CC1A543FCA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED7E604-27B2-CF4B-8FBC-D66C76E4591C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="100" windowWidth="21980" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="100" windowWidth="26100" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diets" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="11">
   <si>
     <t>Diet</t>
   </si>
@@ -59,6 +59,12 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>What the data tells us about the two diets is that the mean weightloss for Diet A is 5.341, and the mean weightloss for Diet B is 3.710. From the supplied data this indicates that those subjects on Diet A have a greater weight reduction than those on Diet B. The standard deviation of Diet B is greater than the standard deviation of Diet A. This indicates that Diet A has less deviation than that of Diet B, and from this we can conclude that the results for diet A's data are more valid.</t>
+  </si>
 </sst>
 </file>
 
@@ -81,6 +87,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -109,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +136,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,34 +478,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="8" max="8" width="28.83203125" customWidth="1"/>
+    <col min="8" max="8" width="82.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="70">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>3.7090000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -512,7 +529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -527,7 +544,7 @@
         <v>5.3411999999999988</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -542,7 +559,7 @@
         <v>2.5356026132351492</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -550,7 +567,7 @@
         <v>9.077</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -558,7 +575,7 @@
         <v>6.4130000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -566,7 +583,7 @@
         <v>5.8769999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -574,7 +591,7 @@
         <v>2.5720000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -582,7 +599,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -590,7 +607,7 @@
         <v>6.8810000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -598,7 +615,7 @@
         <v>7.2649999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -606,7 +623,7 @@
         <v>3.4769999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -614,7 +631,7 @@
         <v>3.7549999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -622,7 +639,7 @@
         <v>8.76</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>